<commit_message>
create_schedule() now sorta works. It renders the html with all the triggers for all the upcoming events, but it still displays a bit weirdly in the pdf output
</commit_message>
<xml_diff>
--- a/haawks-indicator-shortlist (copy).xlsx
+++ b/haawks-indicator-shortlist (copy).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="514">
   <si>
     <t xml:space="preserve">Indicator</t>
   </si>
@@ -1769,8 +1769,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y52" activeCellId="0" sqref="Y52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8056,6 +8056,9 @@
       <c r="D80" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="G80" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J80" s="1" t="n">
         <v>49</v>
       </c>
@@ -8118,6 +8121,9 @@
       <c r="D81" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="G81" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J81" s="1" t="n">
         <v>41</v>
       </c>
@@ -8180,6 +8186,9 @@
       <c r="D82" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="G82" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J82" s="1" t="n">
         <v>42</v>
       </c>
@@ -8242,6 +8251,9 @@
       <c r="D83" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="G83" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J83" s="1" t="n">
         <v>17</v>
       </c>
@@ -8304,6 +8316,9 @@
       <c r="D84" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G84" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="J84" s="1" t="n">
         <v>71</v>
       </c>
@@ -8366,6 +8381,9 @@
       <c r="D85" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G85" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="J85" s="1" t="n">
         <v>72</v>
       </c>
@@ -8428,6 +8446,9 @@
       <c r="D86" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G86" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J86" s="1" t="n">
         <v>57</v>
       </c>
@@ -8490,6 +8511,9 @@
       <c r="D87" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G87" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J87" s="1" t="n">
         <v>58</v>
       </c>
@@ -8552,6 +8576,9 @@
       <c r="D88" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G88" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J88" s="1" t="n">
         <v>59</v>
       </c>
@@ -8614,6 +8641,9 @@
       <c r="D89" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G89" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J89" s="1" t="n">
         <v>51</v>
       </c>
@@ -8676,6 +8706,9 @@
       <c r="D90" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G90" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J90" s="1" t="n">
         <v>52</v>
       </c>
@@ -8738,6 +8771,9 @@
       <c r="D91" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G91" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J91" s="1" t="n">
         <v>53</v>
       </c>
@@ -8800,6 +8836,9 @@
       <c r="D92" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="G92" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J92" s="1" t="n">
         <v>54</v>
       </c>
@@ -8862,6 +8901,9 @@
       <c r="D93" s="1" t="s">
         <v>490</v>
       </c>
+      <c r="G93" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J93" s="1" t="n">
         <v>141</v>
       </c>
@@ -8985,6 +9027,9 @@
       </c>
       <c r="D95" s="1" t="s">
         <v>507</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="J95" s="1" t="n">
         <v>13</v>

</xml_diff>